<commit_message>
refactored the data into a new directory
</commit_message>
<xml_diff>
--- a/K3Fitness_TwosidedNIKKEILO.xlsx
+++ b/K3Fitness_TwosidedNIKKEILO.xlsx
@@ -497,64 +497,64 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1678866623857618</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.1935550714887735</v>
+        <v>-0.1748153949307012</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.170453939667295</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1727477127267293</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.1917399012889055</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.178677714881075</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.1746327438469868</v>
+        <v>-0.174371191312673</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.1893380997431008</v>
+        <v>-0.1622525240592109</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.1869648170073765</v>
+        <v>-0.1682750951017979</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.201868436201968</v>
+        <v>-0.1622525240592109</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.185221851342003</v>
+        <v>-0.1682750951017979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>